<commit_message>
Added initial testing for login Controller
My first real foray into using Xunit so progress is slow. Also made a couple of changes to documentation, I guess.
</commit_message>
<xml_diff>
--- a/documentation/Sprint3Backlog.xlsx
+++ b/documentation/Sprint3Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsacand2\Desktop\Capstone\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nic\source\repos\Ticketmaster\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC8EEBB-4FB1-4079-A57F-6CEFFD096400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FCC087-E81B-4F82-A7EF-B7F63678D0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{0B878F5D-C7DD-43CB-A907-93C9ED087A79}"/>
+    <workbookView xWindow="3495" yWindow="2715" windowWidth="21600" windowHeight="11385" xr2:uid="{0B878F5D-C7DD-43CB-A907-93C9ED087A79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +626,7 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -656,23 +656,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7988135c-1687-4c92-8d73-74afc0a38fa2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010078ED1572585FAA47800541677BB57EC7" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9b42276c791eaef906705969f8eb6749">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7988135c-1687-4c92-8d73-74afc0a38fa2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32983e1bc41a530783be6306a8fc83ab" ns3:_="">
     <xsd:import namespace="7988135c-1687-4c92-8d73-74afc0a38fa2"/>
@@ -828,31 +811,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7988135c-1687-4c92-8d73-74afc0a38fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A7647F-D0D4-43E8-8FCD-E19480B2EF12}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ACAE1C8-90A1-4701-9DA8-417C5E04E17A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7988135c-1687-4c92-8d73-74afc0a38fa2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5576C9E2-D9C8-42DD-BA3F-59DD27B37C4C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -870,6 +846,30 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ACAE1C8-90A1-4701-9DA8-417C5E04E17A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7988135c-1687-4c92-8d73-74afc0a38fa2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A7647F-D0D4-43E8-8FCD-E19480B2EF12}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{8de19331-cc30-459f-8443-6a4b68734b50}" enabled="0" method="" siteId="{8de19331-cc30-459f-8443-6a4b68734b50}" removed="1"/>

</xml_diff>